<commit_message>
Rest Arc Project Start
</commit_message>
<xml_diff>
--- a/DB設計図.xlsx
+++ b/DB設計図.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\JOHO\HIROKI\SpringBoot\workspace2\MyBootApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="46" documentId="13_ncr:1_{C8DD1580-EACC-41D3-97A0-81F98DE47F12}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{92710B1D-49CC-4E2F-B020-BDC04D4BD3D0}"/>
+  <xr:revisionPtr revIDLastSave="60" documentId="13_ncr:1_{C8DD1580-EACC-41D3-97A0-81F98DE47F12}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{AFC4BE34-7CA3-476C-BFF9-E5A3984D16FC}"/>
   <bookViews>
-    <workbookView xWindow="648" yWindow="888" windowWidth="17796" windowHeight="10572" xr2:uid="{B132BA18-7DCD-4A28-908E-A7FA48A3F9DD}"/>
+    <workbookView xWindow="2556" yWindow="840" windowWidth="17796" windowHeight="10716" xr2:uid="{B132BA18-7DCD-4A28-908E-A7FA48A3F9DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="68">
   <si>
     <t>PK</t>
     <phoneticPr fontId="2"/>
@@ -600,6 +600,64 @@
   </si>
   <si>
     <t>→いらんかも</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>いらんかも</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>bool</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>boolean</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>カード</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>or</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>手動</t>
+    </r>
+    <rPh sb="5" eb="7">
+      <t>シュドウ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>rest</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>有給休暇</t>
+    <rPh sb="0" eb="4">
+      <t>ユウキュウキュウカ</t>
+    </rPh>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -607,7 +665,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -663,16 +721,33 @@
       <family val="3"/>
       <charset val="128"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="16">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -887,13 +962,52 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -913,9 +1027,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -961,6 +1072,33 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1277,10 +1415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4248D17-200A-4383-A86F-C9E3D1697F45}">
-  <dimension ref="A1:AQ30"/>
+  <dimension ref="A1:AQ31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
@@ -1303,85 +1441,85 @@
   <sheetData>
     <row r="1" spans="1:12" ht="23.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="2" spans="1:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="10"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="H2" s="8" t="s">
+      <c r="D2" s="9"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="H2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="J2" s="10"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11" t="s">
+      <c r="J2" s="9"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="F3" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="15" t="s">
+      <c r="H3" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="16" t="s">
+      <c r="I3" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="16" t="s">
+      <c r="J3" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="K3" s="16" t="s">
+      <c r="K3" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="L3" s="17" t="s">
+      <c r="L3" s="16" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="E4" s="13"/>
-      <c r="F4" s="14"/>
-      <c r="H4" s="12" t="s">
+      <c r="E4" s="12"/>
+      <c r="F4" s="13"/>
+      <c r="H4" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="I4" s="13" t="s">
+      <c r="I4" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="J4" s="13" t="s">
+      <c r="J4" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="K4" s="13"/>
-      <c r="L4" s="14"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="13"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A5" s="21"/>
+      <c r="A5" s="20"/>
       <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
@@ -1390,7 +1528,7 @@
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
-      <c r="F5" s="22" t="s">
+      <c r="F5" s="21" t="s">
         <v>58</v>
       </c>
       <c r="H5" s="2" t="s">
@@ -1441,7 +1579,7 @@
       </c>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
-      <c r="L7" s="18" t="s">
+      <c r="L7" s="17" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1479,15 +1617,15 @@
       <c r="L9" s="4"/>
     </row>
     <row r="10" spans="1:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="10"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="19" t="s">
+      <c r="D10" s="9"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="18" t="s">
         <v>52</v>
       </c>
       <c r="H10" s="2" t="s">
@@ -1501,19 +1639,19 @@
       <c r="L10" s="4"/>
     </row>
     <row r="11" spans="1:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="E11" s="16" t="s">
+      <c r="E11" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="F11" s="17" t="s">
+      <c r="F11" s="16" t="s">
         <v>5</v>
       </c>
       <c r="H11" s="2" t="s">
@@ -1527,17 +1665,17 @@
       <c r="L11" s="4"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D12" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="E12" s="13"/>
-      <c r="F12" s="14"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="13"/>
       <c r="H12" s="2" t="s">
         <v>20</v>
       </c>
@@ -1549,15 +1687,17 @@
       <c r="L12" s="4"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="4"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="25" t="s">
+        <v>62</v>
+      </c>
       <c r="H13" s="2" t="s">
         <v>34</v>
       </c>
@@ -1570,7 +1710,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B14" s="2" t="s">
         <v>12</v>
       </c>
@@ -1579,22 +1719,22 @@
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
-      <c r="F14" s="18" t="s">
+      <c r="F14" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="H14" s="5" t="s">
+      <c r="H14" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="I14" s="3" t="s">
+      <c r="I14" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="7" t="s">
+      <c r="J14" s="28"/>
+      <c r="K14" s="28"/>
+      <c r="L14" s="29" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B15" s="2" t="s">
         <v>22</v>
       </c>
@@ -1603,8 +1743,19 @@
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
-      <c r="F15" s="18" t="s">
+      <c r="F15" s="17" t="s">
         <v>51</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="30" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.45">
@@ -1624,118 +1775,118 @@
       </c>
     </row>
     <row r="17" spans="1:43" x14ac:dyDescent="0.45">
-      <c r="A17" s="21"/>
       <c r="B17" s="2" t="s">
-        <v>35</v>
+        <v>63</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>26</v>
+        <v>64</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
-      <c r="F17" s="4" t="s">
+      <c r="F17" s="26" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:43" x14ac:dyDescent="0.45">
+      <c r="A18" s="20"/>
+      <c r="B18" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:43" x14ac:dyDescent="0.45">
-      <c r="B18" s="12" t="s">
+    <row r="19" spans="1:43" x14ac:dyDescent="0.45">
+      <c r="B19" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C19" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D18" s="3"/>
-      <c r="E18" s="13" t="s">
+      <c r="D19" s="3"/>
+      <c r="E19" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="F18" s="4"/>
-    </row>
-    <row r="19" spans="1:43" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="20" spans="1:43" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B20" s="8" t="s">
+      <c r="F19" s="4"/>
+    </row>
+    <row r="20" spans="1:43" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="21" spans="1:43" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B21" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C21" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D20" s="10"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11" t="s">
+      <c r="D21" s="9"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="21" spans="1:43" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B21" s="15" t="s">
+    <row r="22" spans="1:43" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B22" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C21" s="16" t="s">
+      <c r="C22" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="D21" s="16" t="s">
+      <c r="D22" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="E21" s="16" t="s">
+      <c r="E22" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="F21" s="17" t="s">
+      <c r="F22" s="16" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:43" x14ac:dyDescent="0.45">
-      <c r="B22" s="12" t="s">
+    <row r="23" spans="1:43" x14ac:dyDescent="0.45">
+      <c r="B23" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C22" s="13" t="s">
+      <c r="C23" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D22" s="13" t="s">
+      <c r="D23" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="E22" s="13"/>
-      <c r="F22" s="14"/>
-    </row>
-    <row r="23" spans="1:43" x14ac:dyDescent="0.45">
-      <c r="B23" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="4" t="s">
-        <v>41</v>
-      </c>
+      <c r="E23" s="12"/>
+      <c r="F23" s="13"/>
     </row>
     <row r="24" spans="1:43" x14ac:dyDescent="0.45">
       <c r="B24" s="2" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:43" x14ac:dyDescent="0.45">
       <c r="B25" s="2" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:43" x14ac:dyDescent="0.45">
       <c r="B26" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>26</v>
@@ -1743,41 +1894,36 @@
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
       <c r="F26" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27" spans="1:43" x14ac:dyDescent="0.45">
       <c r="B27" s="2" t="s">
-        <v>60</v>
+        <v>19</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
       <c r="F27" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="H27" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="AM27"/>
-      <c r="AN27"/>
-      <c r="AO27"/>
-      <c r="AP27"/>
-      <c r="AQ27"/>
+        <v>46</v>
+      </c>
     </row>
     <row r="28" spans="1:43" x14ac:dyDescent="0.45">
       <c r="B28" s="2" t="s">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
       <c r="F28" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
+      </c>
+      <c r="H28" s="20" t="s">
+        <v>61</v>
       </c>
       <c r="AM28"/>
       <c r="AN28"/>
@@ -1786,18 +1932,16 @@
       <c r="AQ28"/>
     </row>
     <row r="29" spans="1:43" x14ac:dyDescent="0.45">
-      <c r="B29" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="C29" s="13" t="s">
-        <v>25</v>
+      <c r="B29" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="D29" s="3"/>
-      <c r="E29" s="13" t="s">
-        <v>37</v>
-      </c>
+      <c r="E29" s="3"/>
       <c r="F29" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="AM29"/>
       <c r="AN29"/>
@@ -1806,11 +1950,31 @@
       <c r="AQ29"/>
     </row>
     <row r="30" spans="1:43" x14ac:dyDescent="0.45">
+      <c r="B30" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D30" s="3"/>
+      <c r="E30" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>48</v>
+      </c>
       <c r="AM30"/>
       <c r="AN30"/>
       <c r="AO30"/>
       <c r="AP30"/>
       <c r="AQ30"/>
+    </row>
+    <row r="31" spans="1:43" x14ac:dyDescent="0.45">
+      <c r="AM31"/>
+      <c r="AN31"/>
+      <c r="AO31"/>
+      <c r="AP31"/>
+      <c r="AQ31"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2"/>

</xml_diff>